<commit_message>
add cai gou kucun zhidao
</commit_message>
<xml_diff>
--- a/db/table.xlsx
+++ b/db/table.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="90" windowWidth="19200" windowHeight="11640"/>
+    <workbookView xWindow="4650" yWindow="90" windowWidth="19200" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="181">
   <si>
     <t>ID</t>
   </si>
@@ -280,10 +280,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>send_status</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>发货状态 0：未发货 1：已发货</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -312,10 +308,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>send_date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>发货时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -389,10 +381,6 @@
   </si>
   <si>
     <t>Table 5: wx_procut   成品配、发、验货主表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Table 6: wx_product_entry   成品配、发、验货详细表（成品库存表）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -699,6 +687,58 @@
   </si>
   <si>
     <t>Table 2: wx_purchase   采购表（食材库存表）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>send_status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>send_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Table 6: wx_product_entry   成品配、发、验货详细表（成品库存表）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wx_product.id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>purchase.id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>decimal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>product_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>purchase_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Table 9: wx_pf_map   成品配、发、验货食材消耗明细表</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -933,7 +973,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -985,32 +1025,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1022,7 +1041,31 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1042,7 +1085,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1084,7 +1127,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1119,7 +1162,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1328,10 +1371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:Q120"/>
+  <dimension ref="B3:Q131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="D129" sqref="D129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1345,17 +1388,17 @@
   <sheetData>
     <row r="3" spans="2:17" ht="196.5" customHeight="1">
       <c r="H3" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="2:17" ht="20.25" customHeight="1">
-      <c r="B8" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
+      <c r="B8" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="2:17" ht="16.5">
       <c r="B9" s="1" t="s">
@@ -1434,7 +1477,7 @@
     <row r="12" spans="2:17" ht="16.5">
       <c r="B12" s="3"/>
       <c r="C12" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1561,13 +1604,13 @@
       <c r="Q19" s="10"/>
     </row>
     <row r="20" spans="2:17" ht="20.25">
-      <c r="B20" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
+      <c r="B20" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
@@ -1711,7 +1754,7 @@
         <v>5</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>21</v>
@@ -1720,7 +1763,7 @@
         <v>13</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>
@@ -1872,14 +1915,14 @@
         <v>14</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>21</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="2:6" ht="16.5">
@@ -1968,13 +2011,13 @@
       </c>
     </row>
     <row r="45" spans="2:6" ht="20.25">
-      <c r="B45" s="17" t="s">
+      <c r="B45" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
     </row>
     <row r="46" spans="2:6" ht="16.5">
       <c r="B46" s="1" t="s">
@@ -2022,7 +2065,7 @@
         <v>9</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="2:6" ht="16.5">
@@ -2039,7 +2082,7 @@
         <v>9</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="2:6" ht="16.5">
@@ -2073,7 +2116,7 @@
         <v>13</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" spans="2:6" ht="16.5">
@@ -2094,13 +2137,13 @@
       </c>
     </row>
     <row r="55" spans="2:6" ht="20.25">
-      <c r="B55" s="17" t="s">
+      <c r="B55" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
     </row>
     <row r="56" spans="2:6" ht="16.5">
       <c r="B56" s="1" t="s">
@@ -2186,13 +2229,13 @@
       </c>
     </row>
     <row r="64" spans="2:6" ht="20.25">
-      <c r="B64" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C64" s="17"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="17"/>
+      <c r="B64" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
     </row>
     <row r="65" spans="2:6" ht="16.5">
       <c r="B65" s="1" t="s">
@@ -2238,7 +2281,7 @@
       </c>
       <c r="E67" s="4"/>
       <c r="F67" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="68" spans="2:6" ht="16.5">
@@ -2291,13 +2334,13 @@
         <v>6</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D71" s="7" t="s">
         <v>50</v>
       </c>
       <c r="F71" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="72" spans="2:6" ht="16.5">
@@ -2305,14 +2348,14 @@
         <v>7</v>
       </c>
       <c r="C72" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D72" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="73" spans="2:6" ht="16.5">
@@ -2320,14 +2363,14 @@
         <v>8</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="2:6" ht="16.5">
@@ -2335,14 +2378,14 @@
         <v>9</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E74" s="4"/>
       <c r="F74" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="75" spans="2:6" ht="16.5">
@@ -2350,14 +2393,14 @@
         <v>10</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>76</v>
+        <v>169</v>
       </c>
       <c r="D75" s="8" t="s">
         <v>21</v>
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="76" spans="2:6" ht="16.5">
@@ -2365,14 +2408,14 @@
         <v>11</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>68</v>
+        <v>168</v>
       </c>
       <c r="D76" s="8" t="s">
         <v>50</v>
       </c>
       <c r="E76" s="4"/>
       <c r="F76" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="77" spans="2:6" ht="16.5">
@@ -2380,14 +2423,14 @@
         <v>12</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D77" s="8" t="s">
         <v>53</v>
       </c>
       <c r="E77" s="4"/>
       <c r="F77" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="78" spans="2:6" ht="16.5">
@@ -2402,14 +2445,14 @@
         <v>13</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D79" s="8" t="s">
         <v>21</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="2:6" ht="16.5">
@@ -2417,14 +2460,14 @@
         <v>14</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D80" s="8" t="s">
         <v>21</v>
       </c>
       <c r="E80" s="4"/>
       <c r="F80" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" spans="2:6" ht="16.5">
@@ -2432,14 +2475,14 @@
         <v>15</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D81" s="8" t="s">
         <v>21</v>
       </c>
       <c r="E81" s="4"/>
       <c r="F81" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="82" spans="2:6" ht="16.5">
@@ -2447,7 +2490,7 @@
         <v>16</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D82" s="8" t="s">
         <v>53</v>
@@ -2475,13 +2518,13 @@
       </c>
     </row>
     <row r="86" spans="2:6" ht="20.25">
-      <c r="B86" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="C86" s="17"/>
-      <c r="D86" s="17"/>
-      <c r="E86" s="17"/>
-      <c r="F86" s="17"/>
+      <c r="B86" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C86" s="18"/>
+      <c r="D86" s="18"/>
+      <c r="E86" s="18"/>
+      <c r="F86" s="18"/>
     </row>
     <row r="87" spans="2:6" ht="16.5">
       <c r="B87" s="1" t="s">
@@ -2520,16 +2563,14 @@
         <v>2</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>59</v>
+        <v>170</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E89" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E89" s="5"/>
       <c r="F89" s="4" t="s">
-        <v>147</v>
+        <v>172</v>
       </c>
     </row>
     <row r="90" spans="2:6" ht="16.5">
@@ -2537,7 +2578,7 @@
         <v>3</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>10</v>
@@ -2546,206 +2587,207 @@
         <v>9</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="91" spans="2:6" ht="16.5">
       <c r="B91" s="3">
-        <v>6</v>
-      </c>
-      <c r="C91" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D91" s="8" t="s">
-        <v>24</v>
+        <v>4</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F91" s="8" t="s">
-        <v>57</v>
+        <v>9</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="92" spans="2:6" ht="16.5">
       <c r="B92" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>33</v>
+        <v>56</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="E92" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F92" s="8" t="s">
-        <v>149</v>
+        <v>57</v>
       </c>
     </row>
     <row r="93" spans="2:6" ht="16.5">
       <c r="B93" s="3">
-        <v>8</v>
-      </c>
-      <c r="C93" s="4" t="s">
-        <v>87</v>
+        <v>6</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E93" s="4">
-        <v>0</v>
-      </c>
-      <c r="F93" s="4" t="s">
-        <v>89</v>
+        <v>33</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F93" s="8" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="94" spans="2:6" ht="16.5">
       <c r="B94" s="3">
-        <v>9</v>
-      </c>
-      <c r="C94" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D94" s="8" t="s">
-        <v>21</v>
+        <v>7</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="E94" s="4">
         <v>0</v>
       </c>
-      <c r="F94" s="8" t="s">
-        <v>94</v>
+      <c r="F94" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="95" spans="2:6" ht="16.5">
       <c r="B95" s="3">
-        <v>10</v>
-      </c>
-      <c r="C95" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D95" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D95" s="8" t="s">
         <v>21</v>
       </c>
       <c r="E95" s="4">
         <v>0</v>
       </c>
-      <c r="F95" s="7" t="s">
+      <c r="F95" s="8" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="96" spans="2:6" ht="16.5">
       <c r="B96" s="3">
-        <v>11</v>
-      </c>
-      <c r="C96" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="D96" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D96" s="8" t="s">
         <v>21</v>
       </c>
       <c r="E96" s="4">
         <v>0</v>
       </c>
-      <c r="F96" s="7" t="s">
-        <v>93</v>
+      <c r="F96" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="97" spans="2:6" ht="16.5">
       <c r="B97" s="3">
-        <v>12</v>
-      </c>
-      <c r="C97" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="D97" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E97" s="16">
+      <c r="C97" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E97" s="4">
         <v>0</v>
       </c>
-      <c r="F97" s="7" t="s">
-        <v>169</v>
+      <c r="F97" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="98" spans="2:6" ht="16.5">
       <c r="B98" s="3">
+        <v>11</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E98" s="4">
+        <v>0</v>
+      </c>
+      <c r="F98" s="8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" ht="16.5">
+      <c r="B99" s="3">
         <v>12</v>
       </c>
-      <c r="C98" s="7" t="s">
+      <c r="C99" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D98" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="F98" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="101" spans="2:6" ht="20.25">
-      <c r="B101" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="C101" s="17"/>
-      <c r="D101" s="17"/>
-      <c r="E101" s="17"/>
-      <c r="F101" s="17"/>
-    </row>
-    <row r="102" spans="2:6" ht="16.5">
-      <c r="B102" s="1" t="s">
+      <c r="D99" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E99" s="9"/>
+      <c r="F99" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" ht="20.25">
+      <c r="B102" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C102" s="18"/>
+      <c r="D102" s="18"/>
+      <c r="E102" s="18"/>
+      <c r="F102" s="18"/>
+    </row>
+    <row r="103" spans="2:6" ht="16.5">
+      <c r="B103" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D102" s="2" t="s">
+      <c r="D103" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E102" s="2" t="s">
+      <c r="E103" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F102" s="2" t="s">
+      <c r="F103" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="103" spans="2:6" ht="16.5">
-      <c r="B103" s="3">
-        <v>1</v>
-      </c>
-      <c r="C103" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D103" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E103" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F103" s="4"/>
     </row>
     <row r="104" spans="2:6" ht="16.5">
       <c r="B104" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E104" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F104" s="4" t="s">
-        <v>147</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F104" s="4"/>
     </row>
     <row r="105" spans="2:6" ht="16.5">
       <c r="B105" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D105" s="4" t="s">
         <v>10</v>
@@ -2754,172 +2796,172 @@
         <v>9</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="106" spans="2:6" ht="16.5">
       <c r="B106" s="3">
-        <v>6</v>
-      </c>
-      <c r="C106" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D106" s="8" t="s">
-        <v>24</v>
+        <v>3</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F106" s="8" t="s">
-        <v>100</v>
+        <v>9</v>
+      </c>
+      <c r="F106" s="4" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="107" spans="2:6" ht="16.5">
       <c r="B107" s="3">
-        <v>8</v>
-      </c>
-      <c r="C107" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D107" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E107" s="4">
-        <v>0</v>
-      </c>
-      <c r="F107" s="4" t="s">
-        <v>98</v>
+        <v>6</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D107" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F107" s="8" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="108" spans="2:6" ht="16.5">
       <c r="B108" s="3">
-        <v>9</v>
-      </c>
-      <c r="C108" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D108" s="8" t="s">
-        <v>21</v>
+        <v>8</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="E108" s="4">
         <v>0</v>
       </c>
-      <c r="F108" s="8" t="s">
-        <v>99</v>
+      <c r="F108" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="109" spans="2:6" ht="16.5">
       <c r="B109" s="3">
-        <v>10</v>
-      </c>
-      <c r="C109" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D109" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E109" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F109" s="7" t="s">
-        <v>103</v>
+        <v>9</v>
+      </c>
+      <c r="C109" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D109" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E109" s="4">
+        <v>0</v>
+      </c>
+      <c r="F109" s="8" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="110" spans="2:6" ht="16.5">
       <c r="B110" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="D110" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E110" s="4">
-        <v>0</v>
+      <c r="E110" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="F110" s="7" t="s">
-        <v>157</v>
+        <v>100</v>
       </c>
     </row>
     <row r="111" spans="2:6" ht="16.5">
       <c r="B111" s="3">
+        <v>11</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D111" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E111" s="4">
+        <v>0</v>
+      </c>
+      <c r="F111" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="112" spans="2:6" ht="16.5">
+      <c r="B112" s="3">
         <v>12</v>
       </c>
-      <c r="C111" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="D111" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="F111" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="114" spans="2:6" ht="20.25">
-      <c r="B114" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="C114" s="17"/>
-      <c r="D114" s="17"/>
-      <c r="E114" s="17"/>
-      <c r="F114" s="17"/>
-    </row>
-    <row r="115" spans="2:6" ht="16.5">
-      <c r="B115" s="1" t="s">
+      <c r="C112" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D112" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="F112" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="115" spans="2:6" ht="20.25">
+      <c r="B115" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="C115" s="18"/>
+      <c r="D115" s="18"/>
+      <c r="E115" s="18"/>
+      <c r="F115" s="18"/>
+    </row>
+    <row r="116" spans="2:6" ht="16.5">
+      <c r="B116" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="C116" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D115" s="2" t="s">
+      <c r="D116" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E115" s="2" t="s">
+      <c r="E116" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F115" s="2" t="s">
+      <c r="F116" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="116" spans="2:6" ht="16.5">
-      <c r="B116" s="3">
-        <v>1</v>
-      </c>
-      <c r="C116" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D116" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E116" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F116" s="4"/>
     </row>
     <row r="117" spans="2:6" ht="16.5">
       <c r="B117" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>163</v>
+        <v>5</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E117" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F117" s="4" t="s">
-        <v>165</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F117" s="4"/>
     </row>
     <row r="118" spans="2:6" ht="16.5">
       <c r="B118" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D118" s="4" t="s">
         <v>10</v>
@@ -2928,43 +2970,192 @@
         <v>9</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="119" spans="2:6" ht="16.5">
       <c r="B119" s="3">
-        <v>6</v>
-      </c>
-      <c r="C119" s="8" t="s">
-        <v>20</v>
+        <v>3</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>161</v>
       </c>
       <c r="D119" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E119" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F119" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="120" spans="2:6" ht="16.5">
+      <c r="B120" s="3">
+        <v>6</v>
+      </c>
+      <c r="C120" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E120" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F119" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="120" spans="2:6" ht="16.5">
-      <c r="B120" s="3"/>
-      <c r="C120" s="4"/>
-      <c r="D120" s="4"/>
-      <c r="E120" s="4"/>
-      <c r="F120" s="4"/>
+      <c r="F120" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="121" spans="2:6" ht="16.5">
+      <c r="B121" s="3"/>
+      <c r="C121" s="4"/>
+      <c r="D121" s="4"/>
+      <c r="E121" s="4"/>
+      <c r="F121" s="4"/>
+    </row>
+    <row r="122" spans="2:6" ht="16.5">
+      <c r="B122" s="17"/>
+      <c r="C122" s="16"/>
+      <c r="D122" s="16"/>
+      <c r="E122" s="16"/>
+      <c r="F122" s="16"/>
+    </row>
+    <row r="124" spans="2:6" ht="20.25">
+      <c r="B124" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="C124" s="18"/>
+      <c r="D124" s="18"/>
+      <c r="E124" s="18"/>
+      <c r="F124" s="18"/>
+    </row>
+    <row r="125" spans="2:6" ht="16.5">
+      <c r="B125" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="2:6" ht="16.5">
+      <c r="B126" s="3">
+        <v>1</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E126" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F126" s="4"/>
+    </row>
+    <row r="127" spans="2:6" ht="16.5">
+      <c r="B127" s="3">
+        <v>2</v>
+      </c>
+      <c r="C127" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D127" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E127" s="5"/>
+      <c r="F127" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="128" spans="2:6" ht="16.5">
+      <c r="B128" s="3">
+        <v>4</v>
+      </c>
+      <c r="C128" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D128" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E128" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F128" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="129" spans="2:6" ht="16.5">
+      <c r="B129" s="3">
+        <v>5</v>
+      </c>
+      <c r="C129" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E129" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F129" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="130" spans="2:6" ht="16.5">
+      <c r="B130" s="3">
+        <v>6</v>
+      </c>
+      <c r="C130" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E130" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F130" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="131" spans="2:6" ht="16.5">
+      <c r="B131" s="3">
+        <v>7</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D131" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="E131" s="4">
+        <v>0</v>
+      </c>
+      <c r="F131" s="4" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B114:F114"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B86:F86"/>
-    <mergeCell ref="B101:F101"/>
+  <mergeCells count="9">
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="B45:F45"/>
     <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B124:F124"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B86:F86"/>
+    <mergeCell ref="B102:F102"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2986,348 +3177,348 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5">
+      <c r="A2" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="D2" s="13"/>
+      <c r="E2" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="1:6" ht="16.5">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="13" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="16.5">
-      <c r="A2" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="B2" s="26" t="s">
+      <c r="D3" s="13"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="1:6" ht="16.5">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D4" s="13"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="1:6" ht="16.5">
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="26" t="s">
-        <v>145</v>
-      </c>
-      <c r="F2" s="13"/>
-    </row>
-    <row r="3" spans="1:6" ht="16.5">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="13" t="s">
+      <c r="D5" s="13"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:6" ht="16.5">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="13"/>
-    </row>
-    <row r="4" spans="1:6" ht="16.5">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="13" t="s">
+      <c r="D6" s="13"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="1:6" ht="16.5">
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="13"/>
-    </row>
-    <row r="5" spans="1:6" ht="16.5">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="13" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="1:6" ht="16.5">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="13"/>
-    </row>
-    <row r="6" spans="1:6" ht="16.5">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="13" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="1:6" ht="16.5">
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="1:6" ht="16.5">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="13" t="s">
+      <c r="D9" s="13"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="13"/>
+    </row>
+    <row r="10" spans="1:6" ht="21" customHeight="1">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="1:6" ht="16.5">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="1:6" ht="16.5">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="1:6" ht="21" customHeight="1">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="13" t="s">
-        <v>122</v>
-      </c>
       <c r="D10" s="13"/>
-      <c r="E10" s="27"/>
+      <c r="E10" s="20"/>
       <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:6" ht="21" customHeight="1">
-      <c r="A11" s="27"/>
-      <c r="B11" s="28"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="28"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:6" ht="16.5">
-      <c r="A12" s="27"/>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="20"/>
+      <c r="B12" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="1:6" ht="16.5">
+      <c r="A13" s="20"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="13"/>
+    </row>
+    <row r="14" spans="1:6" ht="22.5" customHeight="1">
+      <c r="A14" s="20"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" spans="1:6" ht="33" customHeight="1">
+      <c r="A15" s="20"/>
+      <c r="B15" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" spans="1:6" ht="33" customHeight="1">
+      <c r="A16" s="20"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="29" t="s">
-        <v>158</v>
-      </c>
-      <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="1:6" ht="16.5">
-      <c r="A13" s="27"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="13"/>
-    </row>
-    <row r="14" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A14" s="27"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="13"/>
-    </row>
-    <row r="15" spans="1:6" ht="33" customHeight="1">
-      <c r="A15" s="27"/>
-      <c r="B15" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="1:6" ht="33" customHeight="1">
-      <c r="A16" s="27"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="13" t="s">
-        <v>126</v>
-      </c>
       <c r="D16" s="13"/>
-      <c r="E16" s="28"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:6" ht="20.25" customHeight="1">
-      <c r="A17" s="27"/>
-      <c r="B17" s="24"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
     </row>
     <row r="18" spans="1:6" ht="16.5">
-      <c r="A18" s="27"/>
-      <c r="B18" s="21" t="s">
-        <v>137</v>
+      <c r="A18" s="20"/>
+      <c r="B18" s="22" t="s">
+        <v>134</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D18" s="13"/>
-      <c r="E18" s="29" t="s">
-        <v>160</v>
+      <c r="E18" s="25" t="s">
+        <v>157</v>
       </c>
       <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6" ht="16.5">
-      <c r="A19" s="27"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="13" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D19" s="13"/>
-      <c r="E19" s="27"/>
+      <c r="E19" s="20"/>
       <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:6" ht="16.5">
-      <c r="A20" s="27"/>
-      <c r="B20" s="22"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D20" s="13"/>
-      <c r="E20" s="28"/>
+      <c r="E20" s="21"/>
       <c r="F20" s="13"/>
     </row>
     <row r="21" spans="1:6" ht="16.5">
-      <c r="A21" s="27"/>
-      <c r="B21" s="25"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
     </row>
     <row r="22" spans="1:6" ht="24" customHeight="1">
-      <c r="A22" s="27"/>
-      <c r="B22" s="21" t="s">
-        <v>131</v>
+      <c r="A22" s="20"/>
+      <c r="B22" s="22" t="s">
+        <v>128</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="15" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F22" s="13"/>
     </row>
     <row r="23" spans="1:6" ht="20.25" customHeight="1">
-      <c r="A23" s="27"/>
-      <c r="B23" s="22"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D23" s="13"/>
-      <c r="E23" s="29" t="s">
-        <v>162</v>
+      <c r="E23" s="25" t="s">
+        <v>159</v>
       </c>
       <c r="F23" s="13"/>
     </row>
     <row r="24" spans="1:6" ht="16.5">
-      <c r="A24" s="27"/>
-      <c r="B24" s="22"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="23"/>
       <c r="C24" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D24" s="13"/>
-      <c r="E24" s="28"/>
+      <c r="E24" s="21"/>
       <c r="F24" s="13"/>
     </row>
     <row r="25" spans="1:6" ht="16.5">
-      <c r="A25" s="27"/>
-      <c r="B25" s="22"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="13" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D25" s="13"/>
       <c r="E25" s="15" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F25" s="13"/>
     </row>
     <row r="26" spans="1:6" ht="19.5" customHeight="1">
-      <c r="A26" s="27"/>
-      <c r="B26" s="22"/>
+      <c r="A26" s="20"/>
+      <c r="B26" s="23"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
     </row>
     <row r="27" spans="1:6" ht="21" customHeight="1">
-      <c r="A27" s="27"/>
-      <c r="B27" s="21" t="s">
-        <v>136</v>
+      <c r="A27" s="20"/>
+      <c r="B27" s="22" t="s">
+        <v>133</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D27" s="13"/>
-      <c r="E27" s="29" t="s">
-        <v>161</v>
+      <c r="E27" s="25" t="s">
+        <v>158</v>
       </c>
       <c r="F27" s="13"/>
     </row>
     <row r="28" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A28" s="27"/>
-      <c r="B28" s="22"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="23"/>
       <c r="C28" s="13" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D28" s="13"/>
-      <c r="E28" s="27"/>
+      <c r="E28" s="20"/>
       <c r="F28" s="13"/>
     </row>
     <row r="29" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A29" s="27"/>
-      <c r="B29" s="25"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="24"/>
       <c r="C29" s="13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D29" s="13"/>
-      <c r="E29" s="28"/>
+      <c r="E29" s="21"/>
       <c r="F29" s="13"/>
     </row>
     <row r="30" spans="1:6" ht="16.5">
-      <c r="A30" s="27"/>
-      <c r="B30" s="21"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="22"/>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
     </row>
     <row r="31" spans="1:6" ht="16.5">
-      <c r="A31" s="27"/>
-      <c r="B31" s="22"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="23"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
     </row>
     <row r="32" spans="1:6" ht="16.5">
-      <c r="A32" s="27"/>
-      <c r="B32" s="22"/>
+      <c r="A32" s="20"/>
+      <c r="B32" s="23"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
     </row>
     <row r="33" spans="1:6" ht="16.5">
-      <c r="A33" s="28"/>
-      <c r="B33" s="25"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="24"/>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
       <c r="E33" s="13"/>
@@ -3335,6 +3526,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B2:B11"/>
     <mergeCell ref="E2:E11"/>
     <mergeCell ref="B22:B26"/>
     <mergeCell ref="B27:B29"/>
@@ -3345,11 +3541,6 @@
     <mergeCell ref="E18:E20"/>
     <mergeCell ref="E27:E29"/>
     <mergeCell ref="E23:E24"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B2:B11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>